<commit_message>
mrp added why though
</commit_message>
<xml_diff>
--- a/assets/products.xlsx
+++ b/assets/products.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\motobill\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mail\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8634E54E-49A6-4B20-BF72-D6C3131E419B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CC78A8-9620-4C08-9089-BE75948F41A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F4456086-FAE9-4D3D-8AFD-C88EABCCCD98}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>selling_price</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>included_tax</t>
+  </si>
+  <si>
+    <t>mrp</t>
   </si>
 </sst>
 </file>
@@ -112,12 +115,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +438,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,8 +448,8 @@
     <col min="3" max="3" width="17.21875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.21875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.21875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -468,8 +471,10 @@
       <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="G1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="5"/>
       <c r="I1" t="s">
         <v>5</v>
       </c>
@@ -478,8 +483,8 @@
       <c r="D8" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QTXFyd7YaYxsnu+h1wXF0D6HFHUfO/eFzNST4kAOirBD8k3Sasv0d3RB62cJtoT3+3YVQS7pQmKCDDTFUCAMsg==" saltValue="Uhf31ho81sqqXBO/M0p5Ig==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <dataValidations count="4">
+  <sheetProtection algorithmName="SHA-512" hashValue="SiXh3C+mPPbczq5OxnKo0aZaP/BnAkPoy5cF+fPMj54uunWw82hyV0f846iU6w/V7tqN7CoGZdt2MtdylQToyg==" saltValue="98Dx2Ry7BouU6J2fbw+RTA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="5">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not Valid HSN Code" error="HSN Code must be 6 or 8 Digits." sqref="C2:C1048576" xr:uid="{061681B2-514A-49FA-A7AE-71376D09EBAC}">
       <formula1>AND(ISNUMBER(C2), OR(LEN(TEXT(C2,"0"))=6, LEN(TEXT(C2,"0"))=8))</formula1>
     </dataValidation>
@@ -492,6 +497,9 @@
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not Valid Selling Price" error="Selling Price Must be &gt;0" sqref="E2:E7 E9:E1048576 D8" xr:uid="{58109AA0-1F82-469A-A610-ADE0DB7D2A37}">
       <formula1>0</formula1>
     </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{15EB2E3A-B975-4F99-ABD8-A2D993E834EE}">
+      <formula1>0</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>